<commit_message>
version ok avec token
</commit_message>
<xml_diff>
--- a/tests/3_test_data.xlsx
+++ b/tests/3_test_data.xlsx
@@ -35628,7 +35628,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 170/220G CAT.I PLATEAU 1RG_S+1</t>
+          <t>PRIX EXP POMME GOLDEN FRANCE 136/200G CAT.I CAISSE_S+1</t>
         </is>
       </c>
     </row>
@@ -35658,77 +35658,77 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.370000004768372</v>
+        <v>0.9100000262260437</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.389999985694885</v>
+        <v>0.8999999761581421</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.370000004768372</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.320000052452087</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.350000023841858</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.350000023841858</v>
+        <v>1.149999976158142</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.289999961853027</v>
+        <v>0.9700000286102295</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.289999961853027</v>
+        <v>1.100000023841858</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.289999961853027</v>
+        <v>1.179999947547913</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.259999990463257</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.279999971389771</v>
+        <v>1.240000009536743</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="25">
@@ -35756,7 +35756,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 170/220G CAT.I PLATEAU 1RG_S+2</t>
+          <t>PRIX EXP POMME GOLDEN FRANCE 136/200G CAT.I CAISSE_S+2</t>
         </is>
       </c>
     </row>
@@ -35783,77 +35783,77 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.370000004768372</v>
+        <v>0.9100000262260437</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.389999985694885</v>
+        <v>0.8999999761581421</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.370000004768372</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.320000052452087</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.350000023841858</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.350000023841858</v>
+        <v>1.149999976158142</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.289999961853027</v>
+        <v>0.9700000286102295</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.289999961853027</v>
+        <v>1.100000023841858</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.289999961853027</v>
+        <v>1.179999947547913</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.259999990463257</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.279999971389771</v>
+        <v>1.240000009536743</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="24">
@@ -35884,7 +35884,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 170/220G CAT.I PLATEAU 1RG_S+3</t>
+          <t>PRIX EXP POMME GOLDEN FRANCE 136/200G CAT.I CAISSE_S+3</t>
         </is>
       </c>
     </row>
@@ -35908,77 +35908,77 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.370000004768372</v>
+        <v>0.9100000262260437</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.389999985694885</v>
+        <v>0.8999999761581421</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.370000004768372</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.370000004768372</v>
+        <v>1.129999995231628</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.320000052452087</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.350000023841858</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.350000023841858</v>
+        <v>1.149999976158142</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.289999961853027</v>
+        <v>0.9700000286102295</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.289999961853027</v>
+        <v>1.100000023841858</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.289999961853027</v>
+        <v>1.179999947547913</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.259999990463257</v>
+        <v>1.210000038146973</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.279999971389771</v>
+        <v>1.240000009536743</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.279999971389771</v>
+        <v>1.200000047683716</v>
       </c>
     </row>
     <row r="23">

</xml_diff>

<commit_message>
v1 fonctionnelle avec cron
</commit_message>
<xml_diff>
--- a/tests/3_test_data.xlsx
+++ b/tests/3_test_data.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:RN25"/>
+  <dimension ref="A1:RN26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34258,11 +34258,15 @@
       <c r="K25" t="n">
         <v>2.549999952316284</v>
       </c>
-      <c r="L25" t="inlineStr"/>
+      <c r="L25" t="n">
+        <v>2.305000066757202</v>
+      </c>
       <c r="M25" t="n">
         <v>2.599999904632568</v>
       </c>
-      <c r="N25" t="inlineStr"/>
+      <c r="N25" t="n">
+        <v>2.580000042915344</v>
+      </c>
       <c r="O25" t="n">
         <v>2.920000076293945</v>
       </c>
@@ -34601,13 +34605,13 @@
         <v>1</v>
       </c>
       <c r="ER25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="ES25" t="n">
         <v>1</v>
       </c>
       <c r="ET25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EU25" t="n">
         <v>1</v>
@@ -34958,10 +34962,10 @@
         <v>0.07999992370605469</v>
       </c>
       <c r="JG25" t="n">
-        <v>0</v>
+        <v>-0.1749999523162842</v>
       </c>
       <c r="JH25" t="n">
-        <v>0</v>
+        <v>-0.1449999809265137</v>
       </c>
       <c r="JI25" t="n">
         <v>0.05999994277954102</v>
@@ -34970,10 +34974,10 @@
         <v>0.1099998950958252</v>
       </c>
       <c r="JK25" t="n">
-        <v>0</v>
+        <v>-0.3100000619888306</v>
       </c>
       <c r="JL25" t="n">
-        <v>0</v>
+        <v>-0.2299998998641968</v>
       </c>
       <c r="JM25" t="n">
         <v>0.009999990463256836</v>
@@ -35603,6 +35607,1386 @@
         <v>0</v>
       </c>
       <c r="RN25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B26" t="n">
+        <v>6</v>
+      </c>
+      <c r="C26" t="n">
+        <v>26</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1.834999978542328</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1.990000009536743</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.550000011920929</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3.829999923706055</v>
+      </c>
+      <c r="I26" t="n">
+        <v>2.430000066757202</v>
+      </c>
+      <c r="J26" t="n">
+        <v>2.319999933242798</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="L26" t="n">
+        <v>2.130000114440918</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2.369999885559082</v>
+      </c>
+      <c r="N26" t="n">
+        <v>2.269999980926514</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2.859999895095825</v>
+      </c>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="n">
+        <v>3.450000047683716</v>
+      </c>
+      <c r="R26" t="n">
+        <v>3.575000047683716</v>
+      </c>
+      <c r="S26" t="n">
+        <v>3.625</v>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+      <c r="AC26" t="n">
+        <v>1.330000042915344</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>1.289999961853027</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>1.330000042915344</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>19</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>0.9700000286102295</v>
+      </c>
+      <c r="AH26" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>0.9599999785423279</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>1.404999971389771</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>1.350000023841858</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>0.9300000071525574</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>1.210000038146973</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>1.100000023841858</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>1.394999980926514</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>1.370000004768372</v>
+      </c>
+      <c r="AS26" t="n">
+        <v>21</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>21</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>20</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>1.019999980926514</v>
+      </c>
+      <c r="AW26" t="n">
+        <v>1.269999980926514</v>
+      </c>
+      <c r="AX26" t="n">
+        <v>1.370000004768372</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>1.100000023841858</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>1.200000047683716</v>
+      </c>
+      <c r="BA26" t="inlineStr"/>
+      <c r="BB26" t="n">
+        <v>29.75</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>9.375</v>
+      </c>
+      <c r="BD26" t="inlineStr"/>
+      <c r="BE26" t="inlineStr"/>
+      <c r="BF26" t="n">
+        <v>1.700000007947286</v>
+      </c>
+      <c r="BG26" t="inlineStr"/>
+      <c r="BH26" t="inlineStr"/>
+      <c r="BI26" t="n">
+        <v>1.299999952316284</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>2.475000023841858</v>
+      </c>
+      <c r="BK26" t="n">
+        <v>1.299999952316284</v>
+      </c>
+      <c r="BL26" t="n">
+        <v>1.289999961853027</v>
+      </c>
+      <c r="BM26" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="BN26" t="n">
+        <v>2.200000047683716</v>
+      </c>
+      <c r="BO26" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="BP26" t="n">
+        <v>2.099999904632568</v>
+      </c>
+      <c r="BQ26" t="n">
+        <v>1.350000023841858</v>
+      </c>
+      <c r="BR26" t="inlineStr"/>
+      <c r="BS26" t="n">
+        <v>1.300000031789144</v>
+      </c>
+      <c r="BT26" t="n">
+        <v>1.449999988079071</v>
+      </c>
+      <c r="BU26" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="BV26" t="n">
+        <v>1.899999976158142</v>
+      </c>
+      <c r="BW26" t="n">
+        <v>1.857142840112959</v>
+      </c>
+      <c r="BX26" t="n">
+        <v>1.975000023841858</v>
+      </c>
+      <c r="BY26" t="n">
+        <v>1.429999947547913</v>
+      </c>
+      <c r="BZ26" t="n">
+        <v>1.200000047683716</v>
+      </c>
+      <c r="CA26" t="n">
+        <v>1.600000023841858</v>
+      </c>
+      <c r="CB26" t="n">
+        <v>1.200000002980232</v>
+      </c>
+      <c r="CC26" t="n">
+        <v>1.400000015894572</v>
+      </c>
+      <c r="CD26" t="n">
+        <v>1.649999976158142</v>
+      </c>
+      <c r="CE26" t="n">
+        <v>1.733333309491475</v>
+      </c>
+      <c r="CF26" t="n">
+        <v>1.819999980926514</v>
+      </c>
+      <c r="CG26" t="n">
+        <v>2.099999904632568</v>
+      </c>
+      <c r="CH26" t="n">
+        <v>1.799999952316284</v>
+      </c>
+      <c r="CI26" t="n">
+        <v>1.574999988079071</v>
+      </c>
+      <c r="CJ26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="CK26" t="n">
+        <v>2.225000023841858</v>
+      </c>
+      <c r="CL26" t="n">
+        <v>2</v>
+      </c>
+      <c r="CM26" t="n">
+        <v>2.006249994039536</v>
+      </c>
+      <c r="CN26" t="n">
+        <v>1.675000011920929</v>
+      </c>
+      <c r="CO26" t="n">
+        <v>1.274999976158142</v>
+      </c>
+      <c r="CP26" t="inlineStr"/>
+      <c r="CQ26" t="inlineStr"/>
+      <c r="CR26" t="n">
+        <v>2.600000047683716</v>
+      </c>
+      <c r="CS26" t="n">
+        <v>2.524999976158142</v>
+      </c>
+      <c r="CT26" t="n">
+        <v>2.465000033378601</v>
+      </c>
+      <c r="CU26" t="n">
+        <v>1.600000023841858</v>
+      </c>
+      <c r="CV26" t="inlineStr"/>
+      <c r="CW26" t="n">
+        <v>0.8050000071525574</v>
+      </c>
+      <c r="CX26" t="n">
+        <v>1.100000023841858</v>
+      </c>
+      <c r="CY26" t="n">
+        <v>1.149999976158142</v>
+      </c>
+      <c r="CZ26" t="n">
+        <v>1.399999976158142</v>
+      </c>
+      <c r="DA26" t="n">
+        <v>1.350000023841858</v>
+      </c>
+      <c r="DB26" t="inlineStr"/>
+      <c r="DC26" t="inlineStr"/>
+      <c r="DD26" t="inlineStr"/>
+      <c r="DE26" t="n">
+        <v>2.700000047683716</v>
+      </c>
+      <c r="DF26" t="n">
+        <v>1.600000023841858</v>
+      </c>
+      <c r="DG26" t="n">
+        <v>0.8999999761581421</v>
+      </c>
+      <c r="DH26" t="n">
+        <v>1.299999952316284</v>
+      </c>
+      <c r="DI26" t="n">
+        <v>1.399999976158142</v>
+      </c>
+      <c r="DJ26" t="n">
+        <v>0.8999999761581421</v>
+      </c>
+      <c r="DK26" t="n">
+        <v>1.299999952316284</v>
+      </c>
+      <c r="DL26" t="n">
+        <v>1.450000047683716</v>
+      </c>
+      <c r="DM26" t="inlineStr"/>
+      <c r="DN26" t="inlineStr"/>
+      <c r="DO26" t="inlineStr"/>
+      <c r="DP26" t="inlineStr"/>
+      <c r="DQ26" t="n">
+        <v>10719.824</v>
+      </c>
+      <c r="DR26" t="n">
+        <v>338.4</v>
+      </c>
+      <c r="DS26" t="n">
+        <v>107.356</v>
+      </c>
+      <c r="DT26" t="n">
+        <v>92.06999999999999</v>
+      </c>
+      <c r="DU26" t="inlineStr"/>
+      <c r="DV26" t="inlineStr"/>
+      <c r="DW26" t="inlineStr"/>
+      <c r="DX26" t="inlineStr"/>
+      <c r="DY26" t="inlineStr"/>
+      <c r="DZ26" t="inlineStr"/>
+      <c r="EA26" t="inlineStr"/>
+      <c r="EB26" t="inlineStr"/>
+      <c r="EC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED26" t="n">
+        <v>-0.7124999910593033</v>
+      </c>
+      <c r="EE26" t="n">
+        <v>-6.5</v>
+      </c>
+      <c r="EF26" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="EG26" t="n">
+        <v>70.625</v>
+      </c>
+      <c r="EH26" t="n">
+        <v>87</v>
+      </c>
+      <c r="EI26" t="n">
+        <v>2.287500008940697</v>
+      </c>
+      <c r="EJ26" t="n">
+        <v>4637</v>
+      </c>
+      <c r="EK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="ER26" t="n">
+        <v>1</v>
+      </c>
+      <c r="ES26" t="n">
+        <v>1</v>
+      </c>
+      <c r="ET26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EU26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EV26" t="n">
+        <v>0</v>
+      </c>
+      <c r="EW26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EX26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EY26" t="n">
+        <v>1</v>
+      </c>
+      <c r="EZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="FI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FR26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FS26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FT26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FU26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FV26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FW26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FX26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FY26" t="n">
+        <v>1</v>
+      </c>
+      <c r="FZ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GA26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GD26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GE26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GF26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GH26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GN26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GR26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GS26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GT26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GU26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GV26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GW26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="GY26" t="n">
+        <v>1</v>
+      </c>
+      <c r="GZ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HA26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HB26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HD26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HE26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HF26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HH26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HI26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HR26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HS26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HT26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HU26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HV26" t="n">
+        <v>0</v>
+      </c>
+      <c r="HW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="HX26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HY26" t="n">
+        <v>1</v>
+      </c>
+      <c r="HZ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IA26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="IC26" t="n">
+        <v>1</v>
+      </c>
+      <c r="ID26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IE26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IF26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IG26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="II26" t="n">
+        <v>0</v>
+      </c>
+      <c r="IJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="IK26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IL26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IM26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IO26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IP26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IQ26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IR26" t="n">
+        <v>1</v>
+      </c>
+      <c r="IS26" t="n">
+        <v>-0.09500002861022949</v>
+      </c>
+      <c r="IT26" t="n">
+        <v>0.06000000238418579</v>
+      </c>
+      <c r="IU26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="IV26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="IW26" t="n">
+        <v>-0.1399999856948853</v>
+      </c>
+      <c r="IX26" t="n">
+        <v>-0.1599999666213989</v>
+      </c>
+      <c r="IY26" t="n">
+        <v>-0.07000017166137695</v>
+      </c>
+      <c r="IZ26" t="n">
+        <v>0.05999994277954102</v>
+      </c>
+      <c r="JA26" t="n">
+        <v>-0.05999994277954102</v>
+      </c>
+      <c r="JB26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="JC26" t="n">
+        <v>-0.2699999809265137</v>
+      </c>
+      <c r="JD26" t="n">
+        <v>-0.2400000095367432</v>
+      </c>
+      <c r="JE26" t="n">
+        <v>-0.04999995231628418</v>
+      </c>
+      <c r="JF26" t="n">
+        <v>-0.04999995231628418</v>
+      </c>
+      <c r="JG26" t="n">
+        <v>-0.1749999523162842</v>
+      </c>
+      <c r="JH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JI26" t="n">
+        <v>-0.2300000190734863</v>
+      </c>
+      <c r="JJ26" t="n">
+        <v>-0.2400000095367432</v>
+      </c>
+      <c r="JK26" t="n">
+        <v>-0.3100000619888306</v>
+      </c>
+      <c r="JL26" t="n">
+        <v>-0.5499999523162842</v>
+      </c>
+      <c r="JM26" t="n">
+        <v>-0.06000018119812012</v>
+      </c>
+      <c r="JN26" t="n">
+        <v>-0.03000020980834961</v>
+      </c>
+      <c r="JO26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JR26" t="n">
+        <v>-0.1499998569488525</v>
+      </c>
+      <c r="JS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JT26" t="n">
+        <v>-0.125</v>
+      </c>
+      <c r="JU26" t="n">
+        <v>-0.02499997615814209</v>
+      </c>
+      <c r="JV26" t="n">
+        <v>-0.02499997615814209</v>
+      </c>
+      <c r="JW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="JZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KN26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KO26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KQ26" t="n">
+        <v>0.02999997138977051</v>
+      </c>
+      <c r="KR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KS26" t="n">
+        <v>0.04000008106231689</v>
+      </c>
+      <c r="KT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="KV26" t="n">
+        <v>1</v>
+      </c>
+      <c r="KW26" t="n">
+        <v>-0.05999994277954102</v>
+      </c>
+      <c r="KX26" t="n">
+        <v>0.02000004053115845</v>
+      </c>
+      <c r="KY26" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="KZ26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="LA26" t="n">
+        <v>0.02999997138977051</v>
+      </c>
+      <c r="LB26" t="n">
+        <v>0.03999996185302734</v>
+      </c>
+      <c r="LC26" t="n">
+        <v>-0.1666666666666679</v>
+      </c>
+      <c r="LD26" t="n">
+        <v>0.1499996185302734</v>
+      </c>
+      <c r="LE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="LF26" t="n">
+        <v>0.01999998092651367</v>
+      </c>
+      <c r="LG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="LH26" t="n">
+        <v>0.02999997138977051</v>
+      </c>
+      <c r="LI26" t="n">
+        <v>-0.03999996185302734</v>
+      </c>
+      <c r="LJ26" t="n">
+        <v>0.08000004291534424</v>
+      </c>
+      <c r="LK26" t="n">
+        <v>-0.02999997138977051</v>
+      </c>
+      <c r="LL26" t="n">
+        <v>-0.02999997138977051</v>
+      </c>
+      <c r="LM26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="LN26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="LO26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="LP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="LQ26" t="n">
+        <v>-0.004999995231628418</v>
+      </c>
+      <c r="LR26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="LS26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="LT26" t="n">
+        <v>0.09000003337860107</v>
+      </c>
+      <c r="LU26" t="n">
+        <v>1</v>
+      </c>
+      <c r="LV26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="LW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="LX26" t="n">
+        <v>1</v>
+      </c>
+      <c r="LY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="LZ26" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="MA26" t="n">
+        <v>-0.02999997138977051</v>
+      </c>
+      <c r="MB26" t="n">
+        <v>-0.08000004291534424</v>
+      </c>
+      <c r="MC26" t="n">
+        <v>-0.009999990463256836</v>
+      </c>
+      <c r="MD26" t="n">
+        <v>-0.009999990463256836</v>
+      </c>
+      <c r="ME26" t="n">
+        <v>-0.01999998092651367</v>
+      </c>
+      <c r="MF26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="MG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="ML26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MM26" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="MN26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MO26" t="n">
+        <v>-0.125</v>
+      </c>
+      <c r="MP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MU26" t="n">
+        <v>0.1266666650772095</v>
+      </c>
+      <c r="MV26" t="n">
+        <v>-0.2599999904632568</v>
+      </c>
+      <c r="MW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="MZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="ND26" t="n">
+        <v>-0.3249999284744263</v>
+      </c>
+      <c r="NE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NG26" t="n">
+        <v>-0.02500003576278687</v>
+      </c>
+      <c r="NH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NM26" t="n">
+        <v>-0.07500001192092887</v>
+      </c>
+      <c r="NN26" t="n">
+        <v>0.08333334922790536</v>
+      </c>
+      <c r="NO26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NV26" t="n">
+        <v>0.1833333373069763</v>
+      </c>
+      <c r="NW26" t="n">
+        <v>-0.02499997615814209</v>
+      </c>
+      <c r="NX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="NY26" t="n">
+        <v>-0.04999995231628418</v>
+      </c>
+      <c r="NZ26" t="n">
+        <v>-0.07499998807907104</v>
+      </c>
+      <c r="OA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OC26" t="n">
+        <v>1.702989838037183e-08</v>
+      </c>
+      <c r="OD26" t="n">
+        <v>-0.007142867360796279</v>
+      </c>
+      <c r="OE26" t="n">
+        <v>0.02500003576278687</v>
+      </c>
+      <c r="OF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OJ26" t="n">
+        <v>0.1000000238418579</v>
+      </c>
+      <c r="OK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="ON26" t="n">
+        <v>0.06666669746239973</v>
+      </c>
+      <c r="OO26" t="n">
+        <v>-0.03333334128061916</v>
+      </c>
+      <c r="OP26" t="n">
+        <v>-0.01666665077209473</v>
+      </c>
+      <c r="OQ26" t="n">
+        <v>-0.05000007152557373</v>
+      </c>
+      <c r="OR26" t="n">
+        <v>-0.1499999761581421</v>
+      </c>
+      <c r="OS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OT26" t="n">
+        <v>-0.06666664282480883</v>
+      </c>
+      <c r="OU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OV26" t="n">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="OW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="OZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PA26" t="n">
+        <v>0.02500003576278687</v>
+      </c>
+      <c r="PB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PD26" t="n">
+        <v>0.04999995231628418</v>
+      </c>
+      <c r="PE26" t="n">
+        <v>0.02499997615814209</v>
+      </c>
+      <c r="PF26" t="n">
+        <v>0.1250001192092896</v>
+      </c>
+      <c r="PG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PI26" t="n">
+        <v>-0.01250000298023224</v>
+      </c>
+      <c r="PJ26" t="n">
+        <v>0.08958332737286878</v>
+      </c>
+      <c r="PK26" t="n">
+        <v>-0.02499997615814209</v>
+      </c>
+      <c r="PL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PM26" t="n">
+        <v>0.02499997615814209</v>
+      </c>
+      <c r="PN26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PO26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PS26" t="n">
+        <v>-0.009999990463256836</v>
+      </c>
+      <c r="PT26" t="n">
+        <v>0.03749998807907096</v>
+      </c>
+      <c r="PU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PV26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PW26" t="n">
+        <v>-0.02499997615814209</v>
+      </c>
+      <c r="PX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="PZ26" t="n">
+        <v>-0.1000000238418579</v>
+      </c>
+      <c r="QA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QE26" t="n">
+        <v>-0.05000001192092896</v>
+      </c>
+      <c r="QF26" t="n">
+        <v>-0.07499998807907104</v>
+      </c>
+      <c r="QG26" t="n">
+        <v>0.04999995231628418</v>
+      </c>
+      <c r="QH26" t="n">
+        <v>0.04999995231628418</v>
+      </c>
+      <c r="QI26" t="n">
+        <v>-0.1000000238418579</v>
+      </c>
+      <c r="QJ26" t="n">
+        <v>-0.1000000238418579</v>
+      </c>
+      <c r="QK26" t="n">
+        <v>-0.1000000238418579</v>
+      </c>
+      <c r="QL26" t="n">
+        <v>-0.04999995231628418</v>
+      </c>
+      <c r="QM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QN26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QO26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QP26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QQ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QT26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QU26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QV26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QX26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QY26" t="n">
+        <v>0</v>
+      </c>
+      <c r="QZ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RB26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RD26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RE26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RF26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RH26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RJ26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="RN26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -35617,7 +37001,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35732,7 +37116,12 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="n">
+        <v>1.210000038146973</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -35745,7 +37134,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35857,10 +37246,15 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="n">
+        <v>1.210000038146973</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -35873,7 +37267,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35982,7 +37376,9 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="n">
+        <v>1.210000038146973</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -35990,6 +37386,9 @@
     <row r="25">
       <c r="A25" t="inlineStr"/>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
finalisation version regression 2
</commit_message>
<xml_diff>
--- a/tests/3_test_data.xlsx
+++ b/tests/3_test_data.xlsx
@@ -42058,13 +42058,13 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GALA FRANCE 170/220G CAT.I PLATEAU 1RG_S+1</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.414999961853027</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="3">
@@ -42077,113 +42077,103 @@
       <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1.550000011920929</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="A8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>1.396666646003723</v>
-      </c>
+      <c r="A10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.359999984502792</v>
+        <v>1.470000028610229</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.415000021457672</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.415000021457672</v>
+        <v>1.480000019073486</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.420000016689301</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.420000016689301</v>
+        <v>1.529999971389771</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.400000035762787</v>
+        <v>1.450000047683716</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.410000026226044</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.405000030994415</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.384999990463257</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.384999990463257</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.384999990463257</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.375</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.375</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.389999985694885</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.404999971389771</v>
+        <v>1.389999985694885</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.404999971389771</v>
+        <v>1.370000004768372</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.409999966621399</v>
+        <v>1.330000042915344</v>
       </c>
     </row>
     <row r="28">
@@ -42211,13 +42201,13 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GALA FRANCE 170/220G CAT.I PLATEAU 1RG_S+2</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+2</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.414999961853027</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="3">
@@ -42227,113 +42217,103 @@
       <c r="A4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1.550000011920929</v>
-      </c>
+      <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>1.396666646003723</v>
-      </c>
+      <c r="A9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.359999984502792</v>
+        <v>1.470000028610229</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.415000021457672</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.415000021457672</v>
+        <v>1.480000019073486</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.420000016689301</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.420000016689301</v>
+        <v>1.529999971389771</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.400000035762787</v>
+        <v>1.450000047683716</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.410000026226044</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.405000030994415</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.384999990463257</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.384999990463257</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.384999990463257</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.375</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.375</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.389999985694885</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.404999971389771</v>
+        <v>1.389999985694885</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.404999971389771</v>
+        <v>1.370000004768372</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.409999966621399</v>
+        <v>1.330000042915344</v>
       </c>
     </row>
     <row r="27">
@@ -42364,126 +42344,116 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GALA FRANCE 170/220G CAT.I PLATEAU 1RG_S+3</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.439999997615814</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1.550000011920929</v>
-      </c>
+      <c r="A5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1.5</v>
-      </c>
+      <c r="A6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>1.399999976158142</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>1.396666646003723</v>
-      </c>
+      <c r="A8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.359999984502792</v>
+        <v>1.470000028610229</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.415000021457672</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.415000021457672</v>
+        <v>1.480000019073486</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.420000016689301</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.420000016689301</v>
+        <v>1.529999971389771</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.400000035762787</v>
+        <v>1.450000047683716</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.410000026226044</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.405000030994415</v>
+        <v>1.429999947547913</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.384999990463257</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.384999990463257</v>
+        <v>1.399999976158142</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.384999990463257</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.375</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.375</v>
+        <v>1.350000023841858</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.389999985694885</v>
+        <v>1.360000014305115</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.404999971389771</v>
+        <v>1.389999985694885</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.404999971389771</v>
+        <v>1.370000004768372</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.409999966621399</v>
+        <v>1.330000042915344</v>
       </c>
     </row>
     <row r="26">

</xml_diff>

<commit_message>
Modifications pour utiliser XGBClassifier et ajuster les prédictions
</commit_message>
<xml_diff>
--- a/tests/3_test_data.xlsx
+++ b/tests/3_test_data.xlsx
@@ -42058,126 +42058,144 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+1</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+1_class</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.399999976158142</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.470000028610229</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.480000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.529999971389771</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.450000047683716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.429999947547913</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.429999947547913</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.350000023841858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.399999976158142</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.360000014305115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.350000023841858</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.389999985694885</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.370000004768372</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.330000042915344</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -42201,126 +42219,144 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+2</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+2_class</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.399999976158142</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.470000028610229</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.480000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.529999971389771</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.450000047683716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.429999947547913</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.429999947547913</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.350000023841858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.399999976158142</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.360000014305115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.350000023841858</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.389999985694885</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.370000004768372</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.330000042915344</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -42344,126 +42380,144 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+3</t>
+          <t>PRIX EXP POMME GRANNY FRANCE 201/270G CAT.I PLATEAU 1RG_S+3_class</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1.399999976158142</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1.470000028610229</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1.480000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.529999971389771</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1.450000047683716</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1.429999947547913</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1.429999947547913</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.350000023841858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.399999976158142</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.360000014305115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.350000023841858</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.360000014305115</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.389999985694885</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.370000004768372</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.330000042915344</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>